<commit_message>
add data list parsing and tests
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E0F1B1-4F39-0F46-B313-376912A34E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC79C76-CDB0-0F40-84F2-3FC907A291B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9040" yWindow="7400" windowWidth="30060" windowHeight="16940" activeTab="3" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="4000" yWindow="2000" windowWidth="30560" windowHeight="18780" activeTab="3" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
     <sheet name="FormulaAndRefParsing" sheetId="8" r:id="rId2"/>
     <sheet name="ErrorCasesParsing" sheetId="10" r:id="rId3"/>
-    <sheet name="FrontMatterOnly" sheetId="11" r:id="rId4"/>
-    <sheet name=".NestedDataParsing" sheetId="9" r:id="rId5"/>
-    <sheet name=".lists" sheetId="7" r:id="rId6"/>
+    <sheet name="DataListParsing" sheetId="12" r:id="rId4"/>
+    <sheet name="FrontMatterOnly" sheetId="11" r:id="rId5"/>
+    <sheet name=".NestedDataParsing" sheetId="9" r:id="rId6"/>
+    <sheet name=".lists" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="DataLayotList">'.lists'!$C$2:$C$4</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="91">
   <si>
     <t>passwordHash</t>
   </si>
@@ -289,6 +290,33 @@
   </si>
   <si>
     <t>dataLayout</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>prop1</t>
+  </si>
+  <si>
+    <t>prop2</t>
+  </si>
+  <si>
+    <t>prop3</t>
+  </si>
+  <si>
+    <t>first prop in data list</t>
+  </si>
+  <si>
+    <t>This spreadsheet represents a data list instead of a data table, returned as an object</t>
+  </si>
+  <si>
+    <t>Note no front matter on this sheet</t>
+  </si>
+  <si>
+    <t>prop4</t>
+  </si>
+  <si>
+    <t>{ "my": "dude" }</t>
   </si>
 </sst>
 </file>
@@ -379,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -415,6 +443,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -731,9 +766,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1054,7 +1091,7 @@
       </c>
       <c r="H16" s="2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>ba8ea521-e2c7-4a54-bd90-bc1357b9d435</v>
+        <v>df678291-6a7c-4ed9-aea0-966a48cfdbff</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1093,6 +1130,9 @@
       <c r="H18" s="10" t="s">
         <v>50</v>
       </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="19"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -1113,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DFAE23-AEC5-7049-89FE-89CD900ABF71}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1165,7 @@
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>81</v>
       </c>
@@ -1133,7 +1173,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>66</v>
       </c>
@@ -1146,8 +1186,11 @@
       <c r="D2" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1160,8 +1203,11 @@
       <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -1177,10 +1223,16 @@
         <f>C4+B4</f>
         <v>100</v>
       </c>
+      <c r="E4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:D3" xr:uid="{6C1FC800-2037-2E4D-A47A-F0B08A54EDFC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:E3" xr:uid="{6C1FC800-2037-2E4D-A47A-F0B08A54EDFC}">
       <formula1>DataTypeList</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{AE6DA4B5-5C7A-AF42-B5F8-5DF64CBF690C}">
@@ -1188,12 +1240,13 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16853B8-B19B-5340-B113-FF91073746DD}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
@@ -1265,6 +1318,9 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1280,11 +1336,108 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750A2700-74EC-F941-8165-611CD5E037E2}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{764B2826-1FB1-CC46-91E3-AB08F5F4F4AB}">
+      <formula1>DataLayotList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{23A54118-D1A6-8A45-BA1B-533270AC8DB6}">
+      <formula1>DataTypeList</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A816D5-40A3-5549-8589-AB533AFA409D}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1362,7 +1515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDFBAE-D0B5-F94A-A3A1-C8D39188691C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1376,7 +1529,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
   <dimension ref="A1:C8"/>
   <sheetViews>

</xml_diff>

<commit_message>
better definition of data types
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9195FD-393B-A048-B1C5-A9721E0DB65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56B7734-2C5F-E746-9B14-6D804428FD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="2000" windowWidth="30560" windowHeight="18780" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="33640" yWindow="7800" windowWidth="33480" windowHeight="16940" activeTab="3" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
     <sheet name="FormulaAndRefParsing" sheetId="8" r:id="rId2"/>
-    <sheet name="ErrorCasesParsing" sheetId="10" r:id="rId3"/>
+    <sheet name=".ErrorCasesParsing" sheetId="10" r:id="rId3"/>
     <sheet name="DataListParsing" sheetId="12" r:id="rId4"/>
     <sheet name="FrontMatterOnly" sheetId="11" r:id="rId5"/>
     <sheet name=".NestedDataParsing" sheetId="9" r:id="rId6"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="95">
   <si>
     <t>passwordHash</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>badStringList</t>
+  </si>
+  <si>
+    <t>skip1</t>
+  </si>
+  <si>
+    <t>skip2</t>
   </si>
 </sst>
 </file>
@@ -777,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,7 +1106,7 @@
       </c>
       <c r="H16" s="2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>a70e6f34-28dc-429d-9ff6-4da8b197c93d</v>
+        <v>2565d73c-f2d9-4eba-9f3c-2b3a47a22929</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1258,7 +1264,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1358,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750A2700-74EC-F941-8165-611CD5E037E2}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1439,12 +1445,34 @@
         <v>49</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{764B2826-1FB1-CC46-91E3-AB08F5F4F4AB}">
       <formula1>DataLayotList</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{23A54118-D1A6-8A45-BA1B-533270AC8DB6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B5:B10" xr:uid="{23A54118-D1A6-8A45-BA1B-533270AC8DB6}">
       <formula1>DataTypeList</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Finish row value parsing
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56B7734-2C5F-E746-9B14-6D804428FD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD40385-A601-D044-892C-086807DA90D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33640" yWindow="7800" windowWidth="33480" windowHeight="16940" activeTab="3" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="54440" yWindow="1740" windowWidth="30560" windowHeight="18780" activeTab="4" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
     <sheet name="FormulaAndRefParsing" sheetId="8" r:id="rId2"/>
-    <sheet name=".ErrorCasesParsing" sheetId="10" r:id="rId3"/>
+    <sheet name="ErrorCasesParsing" sheetId="10" r:id="rId3"/>
     <sheet name="DataListParsing" sheetId="12" r:id="rId4"/>
-    <sheet name="FrontMatterOnly" sheetId="11" r:id="rId5"/>
-    <sheet name=".NestedDataParsing" sheetId="9" r:id="rId6"/>
-    <sheet name=".lists" sheetId="7" r:id="rId7"/>
+    <sheet name="RowValueListParsing" sheetId="13" r:id="rId5"/>
+    <sheet name="FrontMatterOnly" sheetId="11" r:id="rId6"/>
+    <sheet name=".NestedDataParsing" sheetId="9" r:id="rId7"/>
+    <sheet name=".lists" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="DataLayotList">'.lists'!$C$2:$C$4</definedName>
-    <definedName name="DataTypeList">'.lists'!$A$2:$A$9</definedName>
+    <definedName name="DataLayouts">'.lists'!$E$2:$E$4</definedName>
+    <definedName name="ListDataTypes">'.lists'!$C$2:$C$15</definedName>
+    <definedName name="TableDataTypes">'.lists'!$A$2:$A$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,14 +46,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="120">
   <si>
     <t>passwordHash</t>
   </si>
   <si>
-    <t>Data Types</t>
-  </si>
-  <si>
     <t>number</t>
   </si>
   <si>
@@ -280,9 +279,6 @@
     <t>percent!</t>
   </si>
   <si>
-    <t>Data Layouts</t>
-  </si>
-  <si>
     <t>dataList</t>
   </si>
   <si>
@@ -328,7 +324,88 @@
     <t>skip1</t>
   </si>
   <si>
-    <t>skip2</t>
+    <t>bad string list</t>
+  </si>
+  <si>
+    <t>badBoolList</t>
+  </si>
+  <si>
+    <t>bad bool list</t>
+  </si>
+  <si>
+    <t>number:list</t>
+  </si>
+  <si>
+    <t>boolean:list</t>
+  </si>
+  <si>
+    <t>date:list</t>
+  </si>
+  <si>
+    <t>password:list</t>
+  </si>
+  <si>
+    <t>json:list</t>
+  </si>
+  <si>
+    <t>uuid:list</t>
+  </si>
+  <si>
+    <t>DataLayoutList</t>
+  </si>
+  <si>
+    <t>TableDataTypes</t>
+  </si>
+  <si>
+    <t>ListDataTypes</t>
+  </si>
+  <si>
+    <t>badUuidList</t>
+  </si>
+  <si>
+    <t>stringList</t>
+  </si>
+  <si>
+    <t>numberList</t>
+  </si>
+  <si>
+    <t>jsonList</t>
+  </si>
+  <si>
+    <t>boolList</t>
+  </si>
+  <si>
+    <t>dateList</t>
+  </si>
+  <si>
+    <t>passwordList</t>
+  </si>
+  <si>
+    <t>uuidList</t>
+  </si>
+  <si>
+    <t>This spreadsheet test row value list parsing</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>pw1</t>
+  </si>
+  <si>
+    <t>pw3</t>
+  </si>
+  <si>
+    <t>"jlist"</t>
   </si>
 </sst>
 </file>
@@ -419,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -457,10 +534,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -784,7 +857,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,34 +872,34 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
         <v>100</v>
@@ -834,10 +907,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -845,70 +918,70 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2">
         <v>-100</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
@@ -917,24 +990,24 @@
         <v>40544</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2">
         <v>9999</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>0</v>
@@ -943,24 +1016,24 @@
         <v>44594</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2">
         <v>9999</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="b">
         <v>0</v>
@@ -969,79 +1042,79 @@
         <v>44594</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2">
         <v>15.1515</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="8">
         <v>12116</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2">
         <v>-2000.1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="8">
         <v>16166</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="8">
         <v>20214</v>
@@ -1050,68 +1123,68 @@
         <v>123</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="11">
         <v>24264</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H16" s="2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>2565d73c-f2d9-4eba-9f3c-2b3a47a22929</v>
+        <v>5d69dbc3-9d1a-434f-90ae-9795947a79ae</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1122,43 +1195,46 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="F18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="H18" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
+      <c r="A19" s="17"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:J8" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A8:H8 B3:B5" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
-      <formula1>DataTypeList</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A8:H8" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
+      <formula1>TableDataTypes</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{41DFCB9E-CA3F-8C4F-97D5-E9B20C0F40BC}">
-      <formula1>DataLayotList</formula1>
+      <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B5" xr:uid="{F00C55E2-108D-2B4C-BEAC-0D86026CCDD6}">
+      <formula1>ListDataTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1171,7 +1247,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1182,49 +1258,49 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2">
         <f>3+4*12</f>
@@ -1239,7 +1315,7 @@
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1248,10 +1324,10 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:E3" xr:uid="{6C1FC800-2037-2E4D-A47A-F0B08A54EDFC}">
-      <formula1>DataTypeList</formula1>
+      <formula1>TableDataTypes</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{AE6DA4B5-5C7A-AF42-B5F8-5DF64CBF690C}">
-      <formula1>DataLayotList</formula1>
+      <formula1>DataLayouts</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1261,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16853B8-B19B-5340-B113-FF91073746DD}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1273,66 +1349,78 @@
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="14">
         <v>45542</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="e">
         <f>1/0</f>
@@ -1343,19 +1431,25 @@
         <v>#REF!</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
+        <v>92</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:D6 B3" xr:uid="{7E599051-098C-074E-B40E-BBA797C69756}">
-      <formula1>DataTypeList</formula1>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 E6:F6" xr:uid="{DB05F5BC-F36E-2E48-89C5-F02C63F77CFF}">
+      <formula1>ListDataTypes</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{4BF1630A-B97B-4F45-9252-140126F1C209}">
-      <formula1>DataLayotList</formula1>
+      <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:D6" xr:uid="{4B64D923-84B3-F64A-BE2F-8D8D2073AA53}">
+      <formula1>TableDataTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1364,60 +1458,60 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750A2700-74EC-F941-8165-611CD5E037E2}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>3</v>
+        <v>80</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
-        <v>83</v>
+      <c r="A5" t="s">
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
-        <v>84</v>
+      <c r="A6" t="s">
+        <v>82</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -1425,55 +1519,44 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{764B2826-1FB1-CC46-91E3-AB08F5F4F4AB}">
-      <formula1>DataLayotList</formula1>
+      <formula1>DataLayouts</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B5:B10" xr:uid="{23A54118-D1A6-8A45-BA1B-533270AC8DB6}">
-      <formula1>DataTypeList</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B5:B9" xr:uid="{23A54118-D1A6-8A45-BA1B-533270AC8DB6}">
+      <formula1>ListDataTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1482,6 +1565,263 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50EA8F2-F5B1-C34E-83C3-8E044D181FD2}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="8">
+        <v>45526</v>
+      </c>
+      <c r="D8" s="8">
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B5:B11" xr:uid="{56B6335E-E410-2E4D-AEEA-2E3498B5B2D2}">
+      <formula1>ListDataTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{8DEF093A-44B3-D143-B8ED-5C9D80C9E337}">
+      <formula1>DataLayouts</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A816D5-40A3-5549-8589-AB533AFA409D}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1501,23 +1841,23 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -1525,10 +1865,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
         <v>100</v>
@@ -1536,27 +1876,27 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{9584BD7C-0C96-6640-8863-10FFAF2B6F89}">
-      <formula1>DataLayotList</formula1>
+      <formula1>DataLayouts</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B5" xr:uid="{A8970483-3F59-9141-839F-F1E3DBF1803C}">
-      <formula1>DataTypeList</formula1>
+      <formula1>ListDataTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1564,7 +1904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDFBAE-D0B5-F94A-A3A1-C8D39188691C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1578,71 +1918,165 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>91</v>
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data list testing done
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD40385-A601-D044-892C-086807DA90D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509D7132-068A-4545-93C7-645A0E5D0197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="54440" yWindow="1740" windowWidth="30560" windowHeight="18780" activeTab="4" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="121">
   <si>
     <t>passwordHash</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>"jlist"</t>
+  </si>
+  <si>
+    <t>pw2</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1182,7 @@
       </c>
       <c r="H16" s="2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>5d69dbc3-9d1a-434f-90ae-9795947a79ae</v>
+        <v>ff65d5bc-7f21-4782-84e3-4e4ce5fee049</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1569,7 +1572,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1697,7 +1700,7 @@
         <v>117</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
Improve name DataList -> DataCollectoion
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E687F0-85EC-5343-8CDB-D295AEB50821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DC76B4-B012-0E4A-A235-9C70D7EB7A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="71300" yWindow="5980" windowWidth="30560" windowHeight="18780" activeTab="7" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="49440" yWindow="4480" windowWidth="30560" windowHeight="18780" activeTab="4" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
     <sheet name="FormulaAndRefParsing" sheetId="8" r:id="rId2"/>
     <sheet name="ErrorCasesParsing" sheetId="10" r:id="rId3"/>
-    <sheet name="DataListParsing" sheetId="12" r:id="rId4"/>
+    <sheet name="DataCollectionParsing" sheetId="12" r:id="rId4"/>
     <sheet name="RowValueListParsing" sheetId="13" r:id="rId5"/>
     <sheet name="FrontMatterOnly" sheetId="11" r:id="rId6"/>
     <sheet name=".NestedDataParsing" sheetId="9" r:id="rId7"/>
@@ -279,9 +279,6 @@
     <t>percent!</t>
   </si>
   <si>
-    <t>dataList</t>
-  </si>
-  <si>
     <t>dataTable</t>
   </si>
   <si>
@@ -409,6 +406,9 @@
   </si>
   <si>
     <t>DataLayouts</t>
+  </si>
+  <si>
+    <t>dataCollection</t>
   </si>
 </sst>
 </file>
@@ -859,9 +859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -875,10 +873,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1182,7 +1180,7 @@
       </c>
       <c r="H16" s="2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>4953d6ad-6eb4-4e2d-ba03-a83f9aee9dab</v>
+        <v>c29fae26-86e5-4f27-a335-73e05fdf9f5e</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1226,7 +1224,7 @@
       <c r="A19" s="17"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:J8" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
@@ -1261,10 +1259,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1281,7 +1279,7 @@
         <v>61</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1318,7 +1316,7 @@
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1354,10 +1352,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1392,13 +1390,13 @@
         <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1412,13 +1410,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1434,13 +1432,13 @@
         <v>#REF!</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1464,17 +1462,17 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1484,13 +1482,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1500,18 +1498,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1522,18 +1520,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -1544,7 +1542,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -1571,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50EA8F2-F5B1-C34E-83C3-8E044D181FD2}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1583,10 +1581,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1596,13 +1594,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1612,30 +1610,30 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1654,10 +1652,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -1677,10 +1675,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="8">
         <v>45526</v>
@@ -1691,38 +1689,38 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
@@ -1844,7 +1842,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>72</v>
@@ -1925,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1938,13 +1936,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1955,7 +1953,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1966,7 +1964,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2014,37 +2012,37 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hate to commit here, funky state, but I need to capture a base upon which to evolve a new idea
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73179E9C-8B0E-A74B-8774-D48A4D60B88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125166B5-CFF6-6640-AB06-059726C71578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14620" yWindow="2260" windowWidth="22860" windowHeight="23600" activeTab="1" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="7380" yWindow="4240" windowWidth="22860" windowHeight="19480" activeTab="3" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
     <sheet name="FormulaAndRefParsing" sheetId="8" r:id="rId2"/>
     <sheet name="ErrorCasesParsing" sheetId="10" r:id="rId3"/>
-    <sheet name="DataCollectionParsing" sheetId="12" r:id="rId4"/>
-    <sheet name="RowValueListParsing" sheetId="13" r:id="rId5"/>
+    <sheet name=".DataCollectionParsing" sheetId="12" r:id="rId4"/>
+    <sheet name=".RowValueListParsing" sheetId="13" r:id="rId5"/>
     <sheet name="FrontMatterOnly" sheetId="11" r:id="rId6"/>
     <sheet name=".NestedDataParsing" sheetId="9" r:id="rId7"/>
     <sheet name=".EmptyRowTesting" sheetId="14" r:id="rId8"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="133">
   <si>
     <t>passwordHash</t>
   </si>
@@ -289,15 +289,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>prop1</t>
-  </si>
-  <si>
-    <t>prop2</t>
-  </si>
-  <si>
-    <t>prop3</t>
-  </si>
-  <si>
     <t>first prop in data list</t>
   </si>
   <si>
@@ -307,9 +298,6 @@
     <t>Note no front matter on this sheet</t>
   </si>
   <si>
-    <t>prop4</t>
-  </si>
-  <si>
     <t>{ "my": "dude" }</t>
   </si>
   <si>
@@ -437,13 +425,34 @@
   </si>
   <si>
     <t>Note: should handle trailing delimeter correectly</t>
+  </si>
+  <si>
+    <t>prop1a</t>
+  </si>
+  <si>
+    <t>prop2a</t>
+  </si>
+  <si>
+    <t>prop3a</t>
+  </si>
+  <si>
+    <t>prop4a</t>
+  </si>
+  <si>
+    <t>prop2b</t>
+  </si>
+  <si>
+    <t>prop2c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single prop </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -470,6 +479,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -527,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -571,6 +587,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1210,7 +1227,7 @@
       </c>
       <c r="H16" s="2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>9f27bdce-683d-49f3-92d7-c9385b34dd16</v>
+        <v>2fdf2e88-bbd8-4ed2-8852-05a69144f9f0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1248,16 +1265,6 @@
       </c>
       <c r="H18" s="10" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1284,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DFAE23-AEC5-7049-89FE-89CD900ABF71}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1353,15 +1360,15 @@
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
-        <v>129</v>
+      <c r="B5" s="19" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1380,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16853B8-B19B-5340-B113-FF91073746DD}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1432,13 +1439,13 @@
         <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1452,13 +1459,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E6" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>95</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1474,14 +1481,30 @@
         <v>#REF!</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -1501,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750A2700-74EC-F941-8165-611CD5E037E2}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1514,7 +1537,7 @@
         <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1530,7 +1553,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1540,18 +1563,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1562,18 +1585,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -1584,13 +1607,72 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1598,7 +1680,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{764B2826-1FB1-CC46-91E3-AB08F5F4F4AB}">
       <formula1>DataLayouts</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B5:B9" xr:uid="{23A54118-D1A6-8A45-BA1B-533270AC8DB6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B5:B9 B11:B13 B15" xr:uid="{23A54118-D1A6-8A45-BA1B-533270AC8DB6}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
   </dataValidations>
@@ -1626,7 +1708,7 @@
         <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1642,7 +1724,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1652,30 +1734,30 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1694,10 +1776,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -1717,10 +1799,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C8" s="8">
         <v>45526</v>
@@ -1731,38 +1813,38 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
@@ -1962,32 +2044,32 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2007,12 +2089,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2037,13 +2119,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2065,7 +2147,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2113,37 +2195,37 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fiiiiinallly got collection parsing done
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175B0928-C7E3-024B-BC41-01E77BCD9882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153EB43B-F5DA-6B49-A3AF-02B19520A3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1640" windowWidth="22860" windowHeight="19480" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="1080" yWindow="1240" windowWidth="22860" windowHeight="19480" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
-    <sheet name=".FormulaAndRefParsing" sheetId="8" r:id="rId2"/>
-    <sheet name=".ErrorCasesParsing" sheetId="10" r:id="rId3"/>
-    <sheet name=".DataCollectionParsing" sheetId="12" r:id="rId4"/>
-    <sheet name=".RowValueListParsing" sheetId="13" r:id="rId5"/>
-    <sheet name=".FrontMatterOnly" sheetId="11" r:id="rId6"/>
+    <sheet name="FormulaAndRefParsing" sheetId="8" r:id="rId2"/>
+    <sheet name="ErrorCasesParsing" sheetId="10" r:id="rId3"/>
+    <sheet name="DataCollectionParsing" sheetId="12" r:id="rId4"/>
+    <sheet name="RowValueListParsing" sheetId="13" r:id="rId5"/>
+    <sheet name="FrontMatterOnly" sheetId="11" r:id="rId6"/>
     <sheet name=".NestedDataParsing" sheetId="9" r:id="rId7"/>
     <sheet name=".EmptyRowTesting" sheetId="14" r:id="rId8"/>
     <sheet name=".lists" sheetId="7" r:id="rId9"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="133">
   <si>
     <t>passwordHash</t>
   </si>
@@ -445,7 +445,7 @@
     <t>prop2c</t>
   </si>
   <si>
-    <t xml:space="preserve">single prop </t>
+    <t>single prop</t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="H16" s="2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>0981f269-23a2-450d-97e5-eb32cbf357bf</v>
+        <v>1fa144a7-1554-4bba-bcd8-67349ece3719</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1295,7 +1295,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1393,7 +1393,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView topLeftCell="B3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1530,7 +1530,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1694,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50EA8F2-F5B1-C34E-83C3-8E044D181FD2}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1866,6 +1866,9 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1875,68 +1878,8 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B5:B11" xr:uid="{56B6335E-E410-2E4D-AEEA-2E3498B5B2D2}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
@@ -1954,7 +1897,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
78 arrango data loader (#91)
* minor naming changes

* Improve option defintion and handling for getDG and createDB

* convert db optoins from enum to strings

* update arango data loader to use new db enum defs

* minor cleanup

* convert enums to string ... goodby enums

* doc and edge loading complete

* graph additions checkpoint

* get scaffolding in place for graph loading

* Improve name DataList -> DataCollectoion

* support termination delimeters

* hate to commit here, funky state, but I need to capture a base upon which to evolve a new idea

* funk check point

* Fiiiiinallly got collection parsing done

* minor tweaks
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509D7132-068A-4545-93C7-645A0E5D0197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153EB43B-F5DA-6B49-A3AF-02B19520A3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54440" yWindow="1740" windowWidth="30560" windowHeight="18780" activeTab="4" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="1080" yWindow="1240" windowWidth="22860" windowHeight="19480" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
     <sheet name="FormulaAndRefParsing" sheetId="8" r:id="rId2"/>
     <sheet name="ErrorCasesParsing" sheetId="10" r:id="rId3"/>
-    <sheet name="DataListParsing" sheetId="12" r:id="rId4"/>
+    <sheet name="DataCollectionParsing" sheetId="12" r:id="rId4"/>
     <sheet name="RowValueListParsing" sheetId="13" r:id="rId5"/>
     <sheet name="FrontMatterOnly" sheetId="11" r:id="rId6"/>
     <sheet name=".NestedDataParsing" sheetId="9" r:id="rId7"/>
-    <sheet name=".lists" sheetId="7" r:id="rId8"/>
+    <sheet name=".EmptyRowTesting" sheetId="14" r:id="rId8"/>
+    <sheet name=".lists" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="DataLayouts">'.lists'!$E$2:$E$4</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="133">
   <si>
     <t>passwordHash</t>
   </si>
@@ -279,9 +280,6 @@
     <t>percent!</t>
   </si>
   <si>
-    <t>dataList</t>
-  </si>
-  <si>
     <t>dataTable</t>
   </si>
   <si>
@@ -291,15 +289,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>prop1</t>
-  </si>
-  <si>
-    <t>prop2</t>
-  </si>
-  <si>
-    <t>prop3</t>
-  </si>
-  <si>
     <t>first prop in data list</t>
   </si>
   <si>
@@ -309,9 +298,6 @@
     <t>Note no front matter on this sheet</t>
   </si>
   <si>
-    <t>prop4</t>
-  </si>
-  <si>
     <t>{ "my": "dude" }</t>
   </si>
   <si>
@@ -351,9 +337,6 @@
     <t>uuid:list</t>
   </si>
   <si>
-    <t>DataLayoutList</t>
-  </si>
-  <si>
     <t>TableDataTypes</t>
   </si>
   <si>
@@ -409,13 +392,67 @@
   </si>
   <si>
     <t>pw2</t>
+  </si>
+  <si>
+    <t>DataLayouts</t>
+  </si>
+  <si>
+    <t>dataCollection</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Goal, deteect and handle rows that the user things is empty, but in reacly is not (spaces), had value that was removed, etc</t>
+  </si>
+  <si>
+    <t>Idea, propname with dot notation to do nested</t>
+  </si>
+  <si>
+    <t>adddress.firstName</t>
+  </si>
+  <si>
+    <t>address.lastName</t>
+  </si>
+  <si>
+    <t>etd</t>
+  </si>
+  <si>
+    <t>For exampe</t>
+  </si>
+  <si>
+    <t>should not be parsed after terminaing delimeter</t>
+  </si>
+  <si>
+    <t>Note: should handle trailing delimeter correectly</t>
+  </si>
+  <si>
+    <t>prop1a</t>
+  </si>
+  <si>
+    <t>prop2a</t>
+  </si>
+  <si>
+    <t>prop3a</t>
+  </si>
+  <si>
+    <t>prop4a</t>
+  </si>
+  <si>
+    <t>prop2b</t>
+  </si>
+  <si>
+    <t>prop2c</t>
+  </si>
+  <si>
+    <t>single prop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -442,6 +479,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -499,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -543,6 +587,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,10 +920,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1182,7 +1227,7 @@
       </c>
       <c r="H16" s="2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>ff65d5bc-7f21-4782-84e3-4e4ce5fee049</v>
+        <v>1fa144a7-1554-4bba-bcd8-67349ece3719</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1223,10 +1268,10 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
+      <c r="A19" s="12"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:J8" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
@@ -1250,7 +1295,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1261,10 +1306,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1281,7 +1326,7 @@
         <v>61</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1318,11 +1363,16 @@
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
+      <c r="A5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1340,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16853B8-B19B-5340-B113-FF91073746DD}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="B3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1354,10 +1404,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1392,13 +1442,13 @@
         <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1412,13 +1462,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1434,14 +1484,30 @@
         <v>#REF!</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -1461,20 +1527,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750A2700-74EC-F941-8165-611CD5E037E2}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1484,13 +1550,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1500,18 +1566,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1522,18 +1588,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -1544,13 +1610,72 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1558,7 +1683,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{764B2826-1FB1-CC46-91E3-AB08F5F4F4AB}">
       <formula1>DataLayouts</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B5:B9" xr:uid="{23A54118-D1A6-8A45-BA1B-533270AC8DB6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B5:B9 B11:B13 B15" xr:uid="{23A54118-D1A6-8A45-BA1B-533270AC8DB6}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
   </dataValidations>
@@ -1569,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50EA8F2-F5B1-C34E-83C3-8E044D181FD2}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1583,10 +1708,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1596,13 +1721,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1612,30 +1737,30 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1654,10 +1779,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -1677,10 +1802,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C8" s="8">
         <v>45526</v>
@@ -1691,38 +1816,38 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
@@ -1741,6 +1866,9 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1750,68 +1878,8 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B5:B11" xr:uid="{56B6335E-E410-2E4D-AEEA-2E3498B5B2D2}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
@@ -1829,7 +1897,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1844,7 +1912,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>72</v>
@@ -1909,24 +1977,83 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDFBAE-D0B5-F94A-A3A1-C8D39188691C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EDB1EB7-F575-DD42-8FCB-DF1A880FE326}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1938,13 +2065,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1955,7 +2082,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1966,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2014,72 +2141,37 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parse and remember referenced uuids
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -1,32 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153EB43B-F5DA-6B49-A3AF-02B19520A3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50E455D-824C-5648-B281-A5A6929DC4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1240" windowWidth="22860" windowHeight="19480" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="29020" yWindow="4260" windowWidth="31940" windowHeight="21480" activeTab="2" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
-    <sheet name="FormulaAndRefParsing" sheetId="8" r:id="rId2"/>
-    <sheet name="ErrorCasesParsing" sheetId="10" r:id="rId3"/>
-    <sheet name="DataCollectionParsing" sheetId="12" r:id="rId4"/>
-    <sheet name="RowValueListParsing" sheetId="13" r:id="rId5"/>
-    <sheet name="FrontMatterOnly" sheetId="11" r:id="rId6"/>
-    <sheet name=".NestedDataParsing" sheetId="9" r:id="rId7"/>
-    <sheet name=".EmptyRowTesting" sheetId="14" r:id="rId8"/>
-    <sheet name=".lists" sheetId="7" r:id="rId9"/>
+    <sheet name=".BasicParsing" sheetId="1" r:id="rId1"/>
+    <sheet name="UuidsRefs" sheetId="17" r:id="rId2"/>
+    <sheet name="UuidLinks" sheetId="18" r:id="rId3"/>
+    <sheet name=".FormulaAndRefParsing" sheetId="8" r:id="rId4"/>
+    <sheet name=".ErrorCasesParsing" sheetId="10" r:id="rId5"/>
+    <sheet name=".DataCollectionParsing" sheetId="12" r:id="rId6"/>
+    <sheet name=".RowValueListParsing" sheetId="13" r:id="rId7"/>
+    <sheet name=".FrontMatterOnly" sheetId="11" r:id="rId8"/>
+    <sheet name=".NestedDataParsing" sheetId="9" r:id="rId9"/>
+    <sheet name=".EmptyRowTesting" sheetId="14" r:id="rId10"/>
+    <sheet name=".lists" sheetId="7" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="DataLayouts">'.lists'!$E$2:$E$4</definedName>
-    <definedName name="ListDataTypes">'.lists'!$C$2:$C$15</definedName>
-    <definedName name="TableDataTypes">'.lists'!$A$2:$A$8</definedName>
+    <definedName name="ListDataTypes">'.lists'!$C$2:$C$16</definedName>
+    <definedName name="TableDataTypes">'.lists'!$A$2:$A$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="148">
   <si>
     <t>passwordHash</t>
   </si>
@@ -446,6 +448,51 @@
   </si>
   <si>
     <t>single prop</t>
+  </si>
+  <si>
+    <t>uuid1</t>
+  </si>
+  <si>
+    <t>uuid3</t>
+  </si>
+  <si>
+    <t>uuid2</t>
+  </si>
+  <si>
+    <t>uuids in this sheet will be auto generated and then referenced as appropraite from other sheets</t>
+  </si>
+  <si>
+    <t>uuid:ref</t>
+  </si>
+  <si>
+    <t>u1:_auto_</t>
+  </si>
+  <si>
+    <t>u2:_auto_</t>
+  </si>
+  <si>
+    <t>u3:_auto_</t>
+  </si>
+  <si>
+    <t>otherUuid</t>
+  </si>
+  <si>
+    <t>UuidsToRef.u1</t>
+  </si>
+  <si>
+    <t>UuidsToRef.u2</t>
+  </si>
+  <si>
+    <t>UuidsToRef.u3</t>
+  </si>
+  <si>
+    <t>ref To Uuid 1</t>
+  </si>
+  <si>
+    <t>ref To Uuid 2</t>
+  </si>
+  <si>
+    <t>ref To Uuid 3</t>
   </si>
 </sst>
 </file>
@@ -543,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -588,6 +635,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1227,7 +1277,7 @@
       </c>
       <c r="H16" s="2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>1fa144a7-1554-4bba-bcd8-67349ece3719</v>
+        <v>502f38d0-4b86-4829-bbee-6cd29386e1ff</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1271,7 +1321,7 @@
       <c r="A19" s="12"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="4">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:J8" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
@@ -1290,7 +1340,385 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EDB1EB7-F575-DD42-8FCB-DF1A880FE326}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21EAC818-BA66-8543-910F-5E661BB5C4D9}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="20"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="20"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="10"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:B6" xr:uid="{97B40701-E772-6A47-8B4A-D92B5B8ED1B4}">
+      <formula1>TableDataTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B2 B4" xr:uid="{45214F8D-3B1B-4541-85F2-0AE769EA3CE3}">
+      <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{086341B6-DE50-DE46-88D9-0853C1FF5F0F}">
+      <formula1>ListDataTypes</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD50D8FB-8F35-B74E-8BD6-3A2C7F96F4D1}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="20"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="20"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{142D1292-8418-F547-9D7A-81F160EE90C7}">
+      <formula1>ListDataTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B2 B4" xr:uid="{039BB59C-D518-6543-ACB2-17D9B61D2B40}">
+      <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:B6" xr:uid="{01CB4B22-4321-DD44-AE04-E5F740BDE447}">
+      <formula1>TableDataTypes</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DFAE23-AEC5-7049-89FE-89CD900ABF71}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1388,7 +1816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16853B8-B19B-5340-B113-FF91073746DD}">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -1525,7 +1953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750A2700-74EC-F941-8165-611CD5E037E2}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -1692,7 +2120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50EA8F2-F5B1-C34E-83C3-8E044D181FD2}">
   <dimension ref="A1:J12"/>
   <sheetViews>
@@ -1892,7 +2320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A816D5-40A3-5549-8589-AB533AFA409D}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1975,7 +2403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDFBAE-D0B5-F94A-A3A1-C8D39188691C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2021,161 +2449,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EDB1EB7-F575-DD42-8FCB-DF1A880FE326}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
wrap up referenced parsing
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABD319F-53AF-8C48-83A8-22AF03C4CDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699B4932-7692-8643-BB41-44B1CE2C5D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34180" yWindow="2300" windowWidth="29140" windowHeight="23760" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8140" yWindow="500" windowWidth="29140" windowHeight="23760" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
     <sheet name="UuidsRefs" sheetId="2" r:id="rId2"/>
     <sheet name="UuidLinks" sheetId="3" r:id="rId3"/>
     <sheet name="FormulaAndRefParsing" sheetId="4" r:id="rId4"/>
-    <sheet name=".ErrorCasesParsing" sheetId="5" r:id="rId5"/>
+    <sheet name="ErrorCasesParsing" sheetId="5" r:id="rId5"/>
     <sheet name="DataCollectionParsing" sheetId="6" r:id="rId6"/>
     <sheet name="RowValueListParsing" sheetId="7" r:id="rId7"/>
     <sheet name="FrontMatterOnly" sheetId="8" r:id="rId8"/>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="H16" s="5" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>00e46789-a176-48a6-941c-97f5fdbd0542</v>
+        <v>1c0adb21-9f7c-40ed-baf5-b2238de74fc0</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1895,7 +1895,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U46" sqref="U46"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add pg parsing (#145)
* minor arango type fixes

* got a start on the pg utils

* poker spreadsheet is parsing

* finished up pg utils

* data loader coming along nicely

* support _null_ as a valid cell entry

* wrap up entire test parsing, handle array inputs

* complete postgres data parser
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-spreadsheet-parsing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699B4932-7692-8643-BB41-44B1CE2C5D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9541E6-99EF-0446-A18B-6D43552B1B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8140" yWindow="500" windowWidth="29140" windowHeight="23760" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30940" yWindow="740" windowWidth="29140" windowHeight="23760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="154">
   <si>
     <t>TableDataTypes</t>
   </si>
@@ -498,6 +498,18 @@
   </si>
   <si>
     <t>UuidsRefs.u3</t>
+  </si>
+  <si>
+    <t>someNulls</t>
+  </si>
+  <si>
+    <t>_null_</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>"all in"</t>
   </si>
 </sst>
 </file>
@@ -993,10 +1005,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1008,7 +1020,7 @@
     <col min="5" max="5" width="21.6640625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1320,51 +1332,77 @@
       </c>
       <c r="H16" s="5" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>1c0adb21-9f7c-40ed-baf5-b2238de74fc0</v>
+        <v>5f63fa07-31e1-4597-89f9-13b2de3b3843</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="19"/>
-    </row>
-    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H19" s="19" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
+    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B5" xr:uid="{28FEB1FE-3D55-4848-903C-D4244F576DD9}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
@@ -1381,23 +1419,51 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1894,7 +1960,7 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>